<commit_message>
IDEFICS-3 Pushing priliminary DPEs and DD.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_IDEFICS_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_IDEFICS_TRACY.xlsx
@@ -1,22 +1,132 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BE3E6C-F533-4E10-869C-649B5115267D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>valueType</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>sex_child</t>
+  </si>
+  <si>
+    <t>Sex of the child</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>decimal</t>
+  </si>
+  <si>
+    <t>isced_max</t>
+  </si>
+  <si>
+    <t>phys_activ</t>
+  </si>
+  <si>
+    <t>atc_who_2010</t>
+  </si>
+  <si>
+    <t>Age[years]</t>
+  </si>
+  <si>
+    <t>Isced level:Maximum of both parents</t>
+  </si>
+  <si>
+    <t>ID of the participant</t>
+  </si>
+  <si>
+    <t>migration_T3</t>
+  </si>
+  <si>
+    <t>Migration status of parents</t>
+  </si>
+  <si>
+    <t>One parent migrant</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Early childhood education (and on-going education or no graduation (yet))</t>
+  </si>
+  <si>
+    <t>Primary education</t>
+  </si>
+  <si>
+    <t>Lower secondary education</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Upper secondary education</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Post-secondary non-tertiary education</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Short-cycle tertiary education</t>
+  </si>
+  <si>
+    <t>Bachelors and higher levels</t>
+  </si>
+  <si>
+    <t>Both parents non-migrant</t>
+  </si>
+  <si>
+    <t>Both parents migrant</t>
+  </si>
+  <si>
+    <t>Physical activity[hours per week]</t>
+  </si>
+  <si>
+    <t>child's drug use,last 7 days - ATC code of drug</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,6 +141,43 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,10 +200,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -64,6 +239,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -110,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +325,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +377,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,33 +570,109 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>valueType</t>
-        </is>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -386,29 +681,228 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="14"/>
+    <col min="3" max="3" width="27.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>variable</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>label</t>
-        </is>
-      </c>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="14">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="15">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="15">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="15">
+        <v>2</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
IDEFICS-3 Physical activity:improvised algori. inserted as sugested until clarification. Edu_level: cat.6 mapped to 7 for now until carification. Physical activity accelerom.:improvised algori. inserted until clarification Vitamin Suppl.:Is undetermined because it better if they generate it themselves.
</commit_message>
<xml_diff>
--- a/analyst/Tracy/rmonize/data_dictionary/DD_IDEFICS_TRACY.xlsx
+++ b/analyst/Tracy/rmonize/data_dictionary/DD_IDEFICS_TRACY.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\use-cases-harmonisation\use-cases-harmonisation\analyst\Tracy\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BE3E6C-F533-4E10-869C-649B5115267D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B71597-8176-4ED1-B2FC-5C748AD6F8F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
   <si>
     <t>index</t>
   </si>
@@ -120,13 +120,94 @@
   </si>
   <si>
     <t>child's drug use,last 7 days - ATC code of drug</t>
+  </si>
+  <si>
+    <t>occupst_1</t>
+  </si>
+  <si>
+    <t>occupst_2</t>
+  </si>
+  <si>
+    <t>Employment status of parent</t>
+  </si>
+  <si>
+    <t>Attend school or university</t>
+  </si>
+  <si>
+    <t>Homemaker</t>
+  </si>
+  <si>
+    <t>Temporary company leave (e.g. maternity or paternity leave)</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Full-time job(30 hrs. or more a week)</t>
+  </si>
+  <si>
+    <t>Part-time job(less than 30 hrs. a week)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Retired(also early retirement)</t>
+  </si>
+  <si>
+    <t>Unemployed,for less than one year</t>
+  </si>
+  <si>
+    <t>Unemployed,for a year or more</t>
+  </si>
+  <si>
+    <t>On welfare(social assistance)</t>
+  </si>
+  <si>
+    <t>SED</t>
+  </si>
+  <si>
+    <t>LPA</t>
+  </si>
+  <si>
+    <t>MPA</t>
+  </si>
+  <si>
+    <t>VPA</t>
+  </si>
+  <si>
+    <t>Average time in vigorous PA (min./day)</t>
+  </si>
+  <si>
+    <t>Avg time in moderate PA (min./day)</t>
+  </si>
+  <si>
+    <t>Avg time in light PA (min./day)</t>
+  </si>
+  <si>
+    <t>Avg Sedentary time (min./day)</t>
+  </si>
+  <si>
+    <t>chdiabet</t>
+  </si>
+  <si>
+    <t>History of Diabetes mellitus (ICD-10 2010 – E14)</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Leisure activity [hours per week]</t>
+  </si>
+  <si>
+    <t>leis_activ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,12 +251,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -200,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -217,9 +292,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -227,11 +299,22 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +685,7 @@
       <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D2" t="s">
@@ -644,54 +727,143 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C10" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D10" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="14"/>
+    <col min="2" max="2" width="9.140625" style="15"/>
     <col min="3" max="3" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -699,7 +871,7 @@
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -710,7 +882,7 @@
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="15">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -721,7 +893,7 @@
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="15">
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -732,7 +904,7 @@
       <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="16">
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -743,7 +915,7 @@
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="16">
         <v>1</v>
       </c>
       <c r="C5" t="s">
@@ -754,7 +926,7 @@
       <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="16">
         <v>2</v>
       </c>
       <c r="C6" t="s">
@@ -765,7 +937,7 @@
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="16">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -776,7 +948,7 @@
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="16">
         <v>4</v>
       </c>
       <c r="C8" t="s">
@@ -787,7 +959,7 @@
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="16">
         <v>5</v>
       </c>
       <c r="C9" t="s">
@@ -798,111 +970,287 @@
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="16">
         <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="16">
+        <v>1</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="16">
+        <v>2</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="16">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="16">
+        <v>4</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="16">
+        <v>5</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="16">
+        <v>6</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="16">
+        <v>7</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="16">
+        <v>8</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="16">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="16">
+        <v>10</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="16">
+        <v>1</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="16">
+        <v>2</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="16">
+        <v>3</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="16">
+        <v>4</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="16">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="16">
+        <v>6</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="16">
+        <v>7</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="16">
+        <v>8</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="16">
+        <v>9</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" s="16">
+        <v>10</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B31" s="17">
         <v>0</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B32" s="17">
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B33" s="17">
         <v>2</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="16">
+        <v>1</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="16">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>